<commit_message>
toots excel final version
</commit_message>
<xml_diff>
--- a/toots.xlsx
+++ b/toots.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E81"/>
+  <dimension ref="A1:E121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2264,6 +2264,918 @@
         </is>
       </c>
     </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>1.118738979035425e+17</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>kacey</t>
+        </is>
+      </c>
+      <c r="D82" s="2" t="n">
+        <v>45326.68293981482</v>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;&lt;a href="https://mspsocial.net/tags/programminglanguages" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;programminglanguages&lt;/span&gt;&lt;/a&gt; take:&lt;br&gt;"async" is good but actually all functions should be async by default unless they are specifically marked "sync". The real problem people have with it is the current convention is backwards.&lt;/p&gt;&lt;p&gt;"Sync functions can only call sync functions" would be way easier to deal with than "async functions can only be called by async functions", despite being implementation equivalent.&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>1.118738978649348e+17</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>ruemaleficent</t>
+        </is>
+      </c>
+      <c r="D83" s="2" t="n">
+        <v>45326.68295138889</v>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;I really need a teeth cleaning and I actually love my dentist but I don't want people that close to my face in this day and age, let alone breathing up into my mouth, so I'll continue to scrape plaque off my teeth with my fingernail and stay home.&lt;/p&gt;&lt;p&gt;&lt;a href="https://kolektiva.social/tags/COVID" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;COVID&lt;/span&gt;&lt;/a&gt; &lt;a href="https://kolektiva.social/tags/pandemic" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;pandemic&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>1.118738978647788e+17</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>freyaandersson</t>
+        </is>
+      </c>
+      <c r="D84" s="2" t="n">
+        <v>45326.68293981482</v>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;It's a Sonic and relaxation Sunday for me :genesis_6_button_controller:&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>1.118738978457222e+17</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>de</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>RBLeipzig</t>
+        </is>
+      </c>
+      <c r="D85" s="2" t="n">
+        <v>45326.68219907407</v>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Werfen wir einen Blick in die Kabine! 👀&lt;/p&gt;&lt;p&gt;&lt;a href="https://twitter.com/hashtag/RBLFCU" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;RBLFCU&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>1.118738978305692e+17</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>TrippyKicka</t>
+        </is>
+      </c>
+      <c r="D86" s="2" t="n">
+        <v>45326.68186342593</v>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;The biggest 🤡 in the Steelers fan base &lt;a href="https://twitter.com/asteelcity58/status/1754157845468303631" rel="nofollow noopener noreferrer" target="_blank"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class=""&gt;twitter.com/asteelcity58/s…&lt;/span&gt;&lt;span class="invisible"&gt;&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>1.118738978115704e+17</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>sv</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>PGKurki</t>
+        </is>
+      </c>
+      <c r="D87" s="2" t="n">
+        <v>45326.68296662037</v>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;FAIL. Försök nr 2 att intervjua en VIP för min bok gick i stöpet. Personen dök inte upp i Zoommötet. Sånt händer i hockey. Nu får jag hoppas att personen vill boka nytt datum. Skam den som ger sig. &lt;a href="https://mastodon.social/tags/f%C3%B6rfattarliv" class="mention hashtag" rel="tag"&gt;#&lt;span&gt;författarliv&lt;/span&gt;&lt;/a&gt; &lt;a href="https://mastodon.social/tags/f%C3%B6rfattare" class="mention hashtag" rel="tag"&gt;#&lt;span&gt;författare&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>1.118738978110297e+17</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>ja</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>risahana</t>
+        </is>
+      </c>
+      <c r="D88" s="2" t="n">
+        <v>45326.68295138889</v>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;にんにくは１個使った&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>1.118738977867532e+17</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>shadowfacts</t>
+        </is>
+      </c>
+      <c r="D89" s="2" t="n">
+        <v>45326.68294219908</v>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>you can tell vision pro really is a "spatial computer", because only real computers get MiniPlayer in ~~iTunes~~ &lt;a href="http://Music.app" rel="nofollow noopener noreferrer" target="_blank"&gt;Music.app&lt;/a&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>1.118738977847231e+17</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>trending</t>
+        </is>
+      </c>
+      <c r="D90" s="2" t="n">
+        <v>45326.68293981482</v>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;&lt;a href="https://mastodon.bot/tags/meshiyosoi" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;meshiyosoi&lt;/span&gt;&lt;/a&gt; is now trending across Mastodon&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>1.118738977519554e+17</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>ja</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>d40fe</t>
+        </is>
+      </c>
+      <c r="D91" s="2" t="n">
+        <v>45326.68292824074</v>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;黒いプレート層中間入れて&lt;br&gt;切り絵で白い層重ねた方が綺麗だったなこれ&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>1.118738977069319e+17</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>marcr</t>
+        </is>
+      </c>
+      <c r="D92" s="2" t="n">
+        <v>45326.68293981482</v>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;&lt;a href="https://social.tchncs.de/tags/WordWeavers" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;WordWeavers&lt;/span&gt;&lt;/a&gt; 3.2. - If your antagonist had to choose something to wear from your wardrobe, what would it be and why?&lt;/p&gt;&lt;p&gt;I don't think we're the same... size.&lt;/p&gt;&lt;p&gt;But he'd probably like some of the outdoor and hiking clothes.&lt;/p&gt;&lt;p&gt;I think he'd also have some fun with the pirate costume that's tucked away in there somewhere. :blobcatpirate:&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>1.118738976251515e+17</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>ja</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>tubamei</t>
+        </is>
+      </c>
+      <c r="D93" s="2" t="n">
+        <v>45326.68291666666</v>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;今回のセールプロテインを1000円ぐらい安く買えてウハウハだった&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>1.118738976120082e+17</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>ja</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>fono</t>
+        </is>
+      </c>
+      <c r="D94" s="2" t="n">
+        <v>45326.68288194444</v>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;February 5, 2024 at 12:22AM 現在、体重計測完了。体重は99.8kg。&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>1.118738975915344e+17</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>de</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>T3Z</t>
+        </is>
+      </c>
+      <c r="D95" s="2" t="n">
+        <v>45326.6829050926</v>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Auf nach Wolkenruh! Ich tanke wieder, darf also wieder die Gegner verspotten und Prügel enstecken, damit der Rest der Gruppe die dicke Krecke verkloppen kann. 🛡️&lt;/p&gt;&lt;p&gt;&lt;a href="https://rollenspiel.social/tags/T3Zblubbert%C3%9CberTES" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;T3ZblubbertÜberTES&lt;/span&gt;&lt;/a&gt; &lt;a href="https://rollenspiel.social/tags/ElderScrollsOnline" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;ElderScrollsOnline&lt;/span&gt;&lt;/a&gt; &lt;a href="https://rollenspiel.social/tags/MMORPG" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;MMORPG&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>1.118738975675636e+17</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>de</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>VfL_Wolfsburg</t>
+        </is>
+      </c>
+      <c r="D96" s="2" t="n">
+        <v>45326.68225694444</v>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;⏸️ Pause in der Volkswagen Arena &lt;/p&gt;&lt;p&gt;&lt;a href="https://twitter.com/hashtag/WOBTSG" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;WOBTSG&lt;/span&gt;&lt;/a&gt; &lt;a href="https://twitter.com/hashtag/VfLWolfsburg" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;VfLWolfsburg&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>1.118738975448175e+17</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>de</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>tsghoffenheim</t>
+        </is>
+      </c>
+      <c r="D97" s="2" t="n">
+        <v>45326.68224537037</v>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Pausenführung! &lt;/p&gt;&lt;p&gt;&lt;a href="https://twitter.com/hashtag/WOBTSG" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;WOBTSG&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>1.118738975296948e+17</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>pt</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>rcdc3</t>
+        </is>
+      </c>
+      <c r="D98" s="2" t="n">
+        <v>45326.6829050926</v>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Em 2024, o Corinthians cai em qual campeonato? &lt;a href="https://ursal.zone/tags/Futebol" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;Futebol&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>1.118738975004627e+17</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>ja</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>saku_mio22</t>
+        </is>
+      </c>
+      <c r="D99" s="2" t="n">
+        <v>45326.6825</v>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;久々すぎて全部新鮮だった　ランド　パレードこんなに真面目に見たの初めてかもしれない　ミニーちゃんはアイドル&lt;span class=""&gt; &lt;a href="https://fedibird.com/@saku_mio22/111873895221752441" rel="nofollow noopener noreferrer" class="" target="_blank"&gt;[添付: 5 枚の画像]&lt;/a&gt;&lt;/span&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>1.118738974831175e+17</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>nl</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>debedachtzamen</t>
+        </is>
+      </c>
+      <c r="D100" s="2" t="n">
+        <v>45326.68289351852</v>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Marco Douma – zonder titel, 2020&lt;/p&gt;&lt;p&gt;&lt;a href="https://mastodon.online/tags/drawing" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;drawing&lt;/span&gt;&lt;/a&gt; &lt;a href="https://mastodon.online/tags/charcoal" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;charcoal&lt;/span&gt;&lt;/a&gt; &lt;a href="https://mastodon.online/tags/rotterdam" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;rotterdam&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>1.118738974777593e+17</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>exame</t>
+        </is>
+      </c>
+      <c r="D101" s="2" t="n">
+        <v>45326.68289351852</v>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Valor do estacionamento de SUVs pode triplicar na capital francesa e parisienses vão às urnas&lt;/p&gt;&lt;p&gt;Confira! 👇&lt;br&gt;&lt;a href="https://exame.com/mundo/valor-do-estacionamento-de-suvs-pode-triplicar-na-capital-francesa-e-parisienses-vao-as-urnas/" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class="ellipsis"&gt;exame.com/mundo/valor-do-estac&lt;/span&gt;&lt;span class="invisible"&gt;ionamento-de-suvs-pode-triplicar-na-capital-francesa-e-parisienses-vao-as-urnas/&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;&lt;p&gt;&lt;a href="https://mastodon.online/tags/Mundo" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;Mundo&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="n">
+        <v>1.118738974127249e+17</v>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>zh</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>chronos</t>
+        </is>
+      </c>
+      <c r="D102" s="2" t="n">
+        <v>45326.68287037037</v>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;今天店里同事有请我吃饭&lt;br&gt;感谢他们，如果是我说不定就让离别这件事很简单的就过去了。分明很在意又有点用力过猛的感觉。我还真的挺别扭的。&lt;br&gt;饭后有一起走一段路。聊天也很愉快。&lt;br&gt;谢谢你们，我遇到了很好的人。&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="n">
+        <v>1.11873897396167e+17</v>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>ja</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>kyoto_np</t>
+        </is>
+      </c>
+      <c r="D103" s="2" t="n">
+        <v>45326.68287037037</v>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;京都市長選挙に松井孝治さんが初当選 西田昌司議員「自民党の問題で薄氷の勝利になると思っていた」 (京都新聞)　&lt;a href="https://www.kyoto-np.co.jp/articles/-/1197392" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;https://www.&lt;/span&gt;&lt;span class="ellipsis"&gt;kyoto-np.co.jp/articles/-/1197&lt;/span&gt;&lt;span class="invisible"&gt;392&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="n">
+        <v>1.118738973940567e+17</v>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>puigreixach</t>
+        </is>
+      </c>
+      <c r="D104" s="2" t="n">
+        <v>45326.68287037037</v>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;_&lt;/p&gt;&lt;p&gt;&lt;a href="https://mastodon.world/tags/SilentSunday" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;SilentSunday&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="n">
+        <v>1.118738973843292e+17</v>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>ja</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>kyoto_np</t>
+        </is>
+      </c>
+      <c r="D105" s="2" t="n">
+        <v>45326.68288194444</v>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;京都市長選、立民の福山哲郎氏「ほんまにうれしい、ほんまにうれしいです」松井孝治さん初当選で (京都新聞)　&lt;a href="https://www.kyoto-np.co.jp/articles/-/1197395" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;https://www.&lt;/span&gt;&lt;span class="ellipsis"&gt;kyoto-np.co.jp/articles/-/1197&lt;/span&gt;&lt;span class="invisible"&gt;395&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="n">
+        <v>1.118738973395718e+17</v>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>zh-TW</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>cxyozn</t>
+        </is>
+      </c>
+      <c r="D106" s="2" t="n">
+        <v>45326.68268518519</v>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;同事打掃的時候翻到一隻捏子口，把他組起來放櫃檯但是我覺得她好像需要吃炸雞所以。&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="n">
+        <v>1.11873897304917e+17</v>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>MLClark</t>
+        </is>
+      </c>
+      <c r="D107" s="2" t="n">
+        <v>45326.6828587963</v>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Today's newsletter offers three anecdotes to contextualize an important reminder:&lt;/p&gt;&lt;p&gt;Sometimes the world just won't give us nice, neat, coherent stories.&lt;/p&gt;&lt;p&gt;Never has before!&lt;/p&gt;&lt;p&gt;So when despairing at the haphazard state of the news, maybe consider these three tales: of messy beginnings (mitochondria!), middles (mince pie mythology!), and endings (Patron Saint outcomes!).&lt;/p&gt;&lt;p&gt;We have so little control over the "story" as a whole.&lt;br&gt;Maybe there's a strength in embracing that, though.&lt;/p&gt;&lt;p&gt;&lt;a href="https://open.substack.com/pub/mlclark/p/on-mitochondria-mince-pies-and-patron?r=1ii76&amp;amp;utm_campaign=post&amp;amp;utm_medium=web&amp;amp;showWelcomeOnShare=true" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class="ellipsis"&gt;open.substack.com/pub/mlclark/&lt;/span&gt;&lt;span class="invisible"&gt;p/on-mitochondria-mince-pies-and-patron?r=1ii76&amp;amp;utm_campaign=post&amp;amp;utm_medium=web&amp;amp;showWelcomeOnShare=true&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="n">
+        <v>1.118738972987193e+17</v>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>nuopKINKclassics</t>
+        </is>
+      </c>
+      <c r="D108" s="2" t="n">
+        <v>45326.68284722222</v>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Nu op KINK 80's: Jam - Going Underground&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="n">
+        <v>1.118738972896873e+17</v>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>rff</t>
+        </is>
+      </c>
+      <c r="D109" s="2" t="n">
+        <v>45326.6828125</v>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Now playing on the radiofreefedi.net comfy channel:&lt;br&gt;&lt;br&gt;Three Pots of Coffee by Mykie Frankenstein &lt;a href="https://haunt.graveyard.boo/@mykie" rel="nofollow noopener noreferrer" target="_blank"&gt;https://haunt.graveyard.boo/@mykie&lt;/a&gt;&lt;br&gt;© used with permission&lt;br&gt;&lt;a href="https://mykiefrankenstein.bandcamp.com" rel="nofollow noopener noreferrer" target="_blank"&gt;https://mykiefrankenstein.bandcamp.com&lt;/a&gt;&lt;br&gt;&lt;br&gt;Tune in now: &lt;a href="https://radiofreefedi.net" rel="nofollow noopener noreferrer" target="_blank"&gt;https://radiofreefedi.net&lt;/a&gt;&lt;br&gt;interact with &lt;span class="h-card"&gt;&lt;a href="https://musician.social/@radiofreefedi" class="u-url mention" rel="nofollow noopener noreferrer" target="_blank"&gt;@&lt;span&gt;radiofreefedi&lt;/span&gt;&lt;/a&gt;&lt;/span&gt;&lt;br&gt;&lt;br&gt;your 24/7 community radio from the fediverse to the universe&lt;br&gt;&lt;a href="https://nowplaying.radiofreefedi.net/tags/rffplays" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;rffPlays&lt;/span&gt;&lt;/a&gt; &lt;a href="https://nowplaying.radiofreefedi.net/tags/rffcomfy" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;rffComfy&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="n">
+        <v>1.118738972865379e+17</v>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>SleeperNFL</t>
+        </is>
+      </c>
+      <c r="D110" s="2" t="n">
+        <v>45326.68223379629</v>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;The Ravens ended up paying Odell Beckham Jr. $16M for one season 👀&lt;/p&gt;&lt;p&gt;The results:&lt;/p&gt;&lt;p&gt;- 35 catches&lt;br&gt;- 565 yards&lt;br&gt;- 3 TDs &lt;/p&gt;&lt;p&gt;$457K per catch 😵‍💫&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="n">
+        <v>1.118738972752067e+17</v>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>nintendoblast</t>
+        </is>
+      </c>
+      <c r="D111" s="2" t="n">
+        <v>45326.6828587963</v>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Plumbers Don’t Wear Ties: Definitive Edition (Switch) chegará a eShop em março&lt;/p&gt;&lt;p&gt;Confira! 👇&lt;br&gt;&lt;a href="https://www.nintendoblast.com.br/feeds/4933141685645312943/comments/default" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;https://www.&lt;/span&gt;&lt;span class="ellipsis"&gt;nintendoblast.com.br/feeds/493&lt;/span&gt;&lt;span class="invisible"&gt;3141685645312943/comments/default&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;&lt;p&gt;&lt;a href="https://mastodon.online/tags/Not%C3%ADcia" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;Notícia&lt;/span&gt;&lt;/a&gt; &lt;a href="https://mastodon.online/tags/Switch" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;Switch&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="n">
+        <v>1.118738972679573e+17</v>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>vozhyk</t>
+        </is>
+      </c>
+      <c r="D112" s="2" t="n">
+        <v>45326.6828587963</v>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Складанасці з прэзерватывамі:&lt;/p&gt;&lt;p&gt;&lt;a href="https://youtu.be/iUfXKiHdHn8" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class=""&gt;youtu.be/iUfXKiHdHn8&lt;/span&gt;&lt;span class="invisible"&gt;&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="n">
+        <v>1.11873897238175e+17</v>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>fr</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>Koopa</t>
+        </is>
+      </c>
+      <c r="D113" s="2" t="n">
+        <v>45326.68283564815</v>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Hello, I'm &lt;a href="https://botsin.space/tags/koopa" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;koopa&lt;/span&gt;&lt;/a&gt;. It's 16 : 23&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="n">
+        <v>1.118738972380524e+17</v>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>ja</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>kyoto_np</t>
+        </is>
+      </c>
+      <c r="D114" s="2" t="n">
+        <v>45326.68284722222</v>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;【速報】京都市長選 京都市右京区の開票結果 最多得票は? (京都新聞)　&lt;a href="https://www.kyoto-np.co.jp/articles/-/1197354" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;https://www.&lt;/span&gt;&lt;span class="ellipsis"&gt;kyoto-np.co.jp/articles/-/1197&lt;/span&gt;&lt;span class="invisible"&gt;354&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="n">
+        <v>1.118738971857126e+17</v>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>Iva852</t>
+        </is>
+      </c>
+      <c r="D115" s="2" t="n">
+        <v>45326.68269675926</v>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;🌿🌞 &lt;/p&gt;&lt;p&gt;&lt;a href="https://sunny.garden/tags/SilentSunday" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;SilentSunday&lt;/span&gt;&lt;/a&gt; &lt;br&gt;&lt;a href="https://sunny.garden/tags/photography" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;photography&lt;/span&gt;&lt;/a&gt; &lt;br&gt;&lt;a href="https://sunny.garden/tags/macro" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;macro&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="n">
+        <v>1.118738971743779e+17</v>
+      </c>
+      <c r="B116" t="inlineStr"/>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>www.numerama.com</t>
+        </is>
+      </c>
+      <c r="D116" s="2" t="n">
+        <v>45326.68284722222</v>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Realme 9 Pro+ 5G : un excellent smartphone milieu de gamme, surtout pendant les soldes&lt;/p&gt;&lt;p&gt;&lt;a href="https://www.numerama.com/tech/1623220-realme-9-pro-5g-un-excellent-smartphone-milieu-de-gamme-surtout-pendant-les-soldes.html" rel="nofollow noopener noreferrer" target="_blank"&gt;www.numerama.com/tech/1623220-realme-9-pro-5g-un-excellent-smartphone-milieu-de-gamme-surtout-pendant-les-soldes.html&lt;/a&gt;&lt;/p&gt;&lt;p&gt;[Deal du jour] Le 9 Pro+ de Realme est un smartphone milieu de gamme qui offre de bonnes performances. Si vous recherchez un appareil pas trop cher et parfait au quotidien, c'est un excellent modèle, surtout durant les soldes.&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="n">
+        <v>1.118738971722608e+17</v>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>de</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>p0lise</t>
+        </is>
+      </c>
+      <c r="D117" s="2" t="n">
+        <v>45326.68283564815</v>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Heute meine erste Rennradrunde des Jahres gedreht. Bin natürlich gleich wieder zigfach zu eng überholt worden. Ich kriege den Gedanken nicht aus dem Kopf, dass ich jederzeit der nächste sein könnte. &lt;a href="https://hessen.social/tags/ripnatenom" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;ripnatenom&lt;/span&gt;&lt;/a&gt;.&lt;/p&gt;&lt;p&gt;Danke für nichts, &lt;span class="h-card" translate="no"&gt;&lt;a href="https://social.bund.de/@bmdv" class="u-url mention" rel="nofollow noopener noreferrer" target="_blank"&gt;@&lt;span&gt;bmdv&lt;/span&gt;&lt;/a&gt;&lt;/span&gt;. Und zeigt jetzt bitte nicht wieder mit dem Finger auf Länder und Kommunen. IHR seid das Bundesministerium für Verkehr. Und ihr schafft es nichtmal, in Sachen &lt;a href="https://hessen.social/tags/stvg" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;stvg&lt;/span&gt;&lt;/a&gt;-Novelle den Vermittlungssausschuss anzurufen.&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="n">
+        <v>1.118738971421618e+17</v>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>de</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>Thomas8998</t>
+        </is>
+      </c>
+      <c r="D118" s="2" t="n">
+        <v>45326.6828484375</v>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Hauseigentümer, die sich über Strompreise beklagen und gleichzeitig, trotz Möglichkeit, keine Fotovoltaik-Anlage betreiben, kann mir jemand diese besondere Spezies erklären?&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="n">
+        <v>1.118738971144983e+17</v>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>ja</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>narutake</t>
+        </is>
+      </c>
+      <c r="D119" s="2" t="n">
+        <v>45326.68283564815</v>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;うわあああああああああああ&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="n">
+        <v>1.118738970487246e+17</v>
+      </c>
+      <c r="B120" t="inlineStr"/>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>HMJN</t>
+        </is>
+      </c>
+      <c r="D120" s="2" t="n">
+        <v>45326.68282489583</v>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;&lt;span&gt;藍ちゃんジャンケンやめたの&lt;/span&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="n">
+        <v>1.118738970206463e+17</v>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>de</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>formschub</t>
+        </is>
+      </c>
+      <c r="D121" s="2" t="n">
+        <v>45326.68271990741</v>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Auf der heutigen Wanderung mitten im Wald lag erst ein großer Strunk frischer Brokkoli am Wegesrand, dann eine Weile später ein großer Haufen einwandfreier Kartoffeln. Scheint, als ballten sich hier in der Gegend die Gemüseverächter.&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>